<commit_message>
validation and excel format
</commit_message>
<xml_diff>
--- a/public/files/user_profiles.xlsx
+++ b/public/files/user_profiles.xlsx
@@ -22,22 +22,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middle_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,6 +254,7 @@
         <v>5</v>
       </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>